<commit_message>
Build up the Details section
Most core functionality is done at this point!

Still need to implement filters, and get Lat/Lon values for all the activities
</commit_message>
<xml_diff>
--- a/public/resources/classes.xlsx
+++ b/public/resources/classes.xlsx
@@ -2079,16 +2079,16 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2199,8 +2199,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ218"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2311,16 +2311,16 @@
       <c r="D3" s="4" t="n">
         <v>43.110947186732</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="4" t="n">
         <v>-88.5022081314075</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>44986</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="7" t="n">
         <v>0.625</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="7" t="n">
         <v>0.6875</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -2357,19 +2357,19 @@
       <c r="F4" s="6" t="n">
         <v>44987</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="G4" s="7" t="n">
         <v>0.625</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="7" t="n">
         <v>0.708333333333333</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="9" t="n">
+      <c r="J4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="8" t="n">
         <v>9</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -2395,22 +2395,22 @@
       <c r="D5" s="4" t="n">
         <v>43.2175946085861</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="4" t="n">
         <v>-88.1452177737315</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>44987</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="9" t="n">
+      <c r="J5" s="8" t="n">
         <v>18</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -2426,7 +2426,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="243.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -2436,21 +2436,25 @@
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="4" t="n">
+        <v>42.886038333602</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>-87.9633897374327</v>
+      </c>
       <c r="F6" s="6" t="n">
         <v>44987</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="8" t="n">
         <v>5</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -2466,7 +2470,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -2476,15 +2480,19 @@
       <c r="C7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="4" t="n">
+        <v>43.3204620708738</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>-88.3820853313831</v>
+      </c>
       <c r="F7" s="6" t="n">
         <v>44988</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="G7" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="H7" s="8" t="n">
+      <c r="H7" s="7" t="n">
         <v>0.5625</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -2521,16 +2529,16 @@
       <c r="F8" s="6" t="n">
         <v>44988</v>
       </c>
-      <c r="G8" s="8" t="n">
+      <c r="G8" s="7" t="n">
         <v>0.625</v>
       </c>
-      <c r="H8" s="8" t="n">
+      <c r="H8" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="9" t="n">
+      <c r="J8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="4" t="s">
@@ -2546,7 +2554,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -2556,24 +2564,28 @@
       <c r="C9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="4" t="n">
+        <v>43.0554104008493</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>-88.1251718044087</v>
+      </c>
       <c r="F9" s="6" t="n">
         <v>44991</v>
       </c>
-      <c r="G9" s="8" t="n">
+      <c r="G9" s="7" t="n">
         <v>0.6875</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>0.75</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="8" t="n">
         <v>10</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -2596,15 +2608,19 @@
       <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="4" t="n">
+        <v>42.9588185809146</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>-87.9783010214933</v>
+      </c>
       <c r="F10" s="6" t="n">
         <v>44991</v>
       </c>
-      <c r="G10" s="8" t="n">
+      <c r="G10" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="H10" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -2626,7 +2642,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="103.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
@@ -2636,15 +2652,19 @@
       <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="4" t="n">
+        <v>42.9588185809146</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>-87.9783010214933</v>
+      </c>
       <c r="F11" s="6" t="n">
         <v>44991</v>
       </c>
-      <c r="G11" s="8" t="n">
+      <c r="G11" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H11" s="8" t="n">
+      <c r="H11" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -2666,7 +2686,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>58</v>
       </c>
@@ -2676,24 +2696,28 @@
       <c r="C12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4" t="n">
+        <v>42.9303830470777</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>-88.0347295890706</v>
+      </c>
       <c r="F12" s="6" t="n">
         <v>44992</v>
       </c>
-      <c r="G12" s="8" t="n">
+      <c r="G12" s="7" t="n">
         <v>0.5625</v>
       </c>
-      <c r="H12" s="8" t="n">
+      <c r="H12" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="9" t="n">
+      <c r="J12" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="11" t="s">
@@ -2706,7 +2730,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
@@ -2716,15 +2740,19 @@
       <c r="C13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="4" t="n">
+        <v>43.0617188452041</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>-88.4146724448863</v>
+      </c>
       <c r="F13" s="6" t="n">
         <v>44992</v>
       </c>
-      <c r="G13" s="8" t="n">
+      <c r="G13" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H13" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -2771,7 +2799,7 @@
       <c r="J14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="9" t="n">
+      <c r="K14" s="8" t="n">
         <v>4</v>
       </c>
       <c r="L14" s="4" t="s">
@@ -2784,7 +2812,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
@@ -2794,15 +2822,19 @@
       <c r="C15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="D15" s="4" t="n">
+        <v>43.4186740415331</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>-88.218165645702</v>
+      </c>
       <c r="F15" s="6" t="n">
         <v>44993</v>
       </c>
-      <c r="G15" s="8" t="n">
+      <c r="G15" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H15" s="8" t="n">
+      <c r="H15" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -2834,15 +2866,19 @@
       <c r="C16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="4" t="n">
+        <v>43.2326552746764</v>
+      </c>
+      <c r="E16" s="9" t="n">
+        <v>-87.9788473160436</v>
+      </c>
       <c r="F16" s="6" t="n">
         <v>44993</v>
       </c>
-      <c r="G16" s="8" t="n">
+      <c r="G16" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H16" s="8" t="n">
+      <c r="H16" s="7" t="n">
         <v>0.604166666666667</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -2879,16 +2915,16 @@
       <c r="F17" s="6" t="n">
         <v>44993</v>
       </c>
-      <c r="G17" s="8" t="n">
+      <c r="G17" s="7" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="H17" s="8" t="n">
+      <c r="H17" s="7" t="n">
         <v>0.854166666666667</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="9" t="n">
+      <c r="J17" s="8" t="n">
         <v>1</v>
       </c>
       <c r="K17" s="4" t="s">
@@ -2904,7 +2940,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="256.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>84</v>
       </c>
@@ -2914,15 +2950,19 @@
       <c r="C18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="D18" s="4" t="n">
+        <v>43.8587608838201</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>-88.2835981620474</v>
+      </c>
       <c r="F18" s="6" t="n">
         <v>44993</v>
       </c>
-      <c r="G18" s="8" t="n">
+      <c r="G18" s="7" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="H18" s="8" t="n">
+      <c r="H18" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I18" s="4" t="s">
@@ -2931,7 +2971,7 @@
       <c r="J18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="K18" s="9" t="n">
+      <c r="K18" s="8" t="n">
         <v>40</v>
       </c>
       <c r="L18" s="13" t="n">
@@ -2944,7 +2984,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>88</v>
       </c>
@@ -2954,15 +2994,19 @@
       <c r="C19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="D19" s="4" t="n">
+        <v>42.9475870367452</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <v>-88.1566877313984</v>
+      </c>
       <c r="F19" s="6" t="n">
         <v>44993</v>
       </c>
-      <c r="G19" s="8" t="n">
+      <c r="G19" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H19" s="8" t="n">
+      <c r="H19" s="7" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -2984,7 +3028,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="358.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>92</v>
       </c>
@@ -2994,15 +3038,19 @@
       <c r="C20" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="D20" s="4" t="n">
+        <v>43.0602032879812</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <v>-88.008941602558</v>
+      </c>
       <c r="F20" s="6" t="n">
         <v>44994</v>
       </c>
-      <c r="G20" s="8" t="n">
+      <c r="G20" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H20" s="8" t="n">
+      <c r="H20" s="7" t="n">
         <v>0.46875</v>
       </c>
       <c r="I20" s="4" t="s">
@@ -3039,10 +3087,10 @@
       <c r="F21" s="6" t="n">
         <v>44995</v>
       </c>
-      <c r="G21" s="8" t="n">
+      <c r="G21" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H21" s="8" t="n">
+      <c r="H21" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I21" s="4" t="s">
@@ -3064,7 +3112,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>100</v>
       </c>
@@ -3074,21 +3122,25 @@
       <c r="C22" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="D22" s="4" t="n">
+        <v>43.3828052241511</v>
+      </c>
+      <c r="E22" s="9" t="n">
+        <v>-87.8701329448732</v>
+      </c>
       <c r="F22" s="6" t="n">
         <v>44995</v>
       </c>
-      <c r="G22" s="8" t="n">
+      <c r="G22" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H22" s="8" t="n">
+      <c r="H22" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="J22" s="9" t="n">
+      <c r="J22" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="4" t="s">
@@ -3119,10 +3171,10 @@
       <c r="F23" s="6" t="n">
         <v>44995</v>
       </c>
-      <c r="G23" s="8" t="n">
+      <c r="G23" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H23" s="8" t="n">
+      <c r="H23" s="7" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="I23" s="4" t="s">
@@ -3144,7 +3196,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>108</v>
       </c>
@@ -3154,24 +3206,28 @@
       <c r="C24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="D24" s="4" t="n">
+        <v>43.0186481784581</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>-87.9471676448881</v>
+      </c>
       <c r="F24" s="6" t="n">
         <v>44995</v>
       </c>
-      <c r="G24" s="8" t="n">
+      <c r="G24" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H24" s="8" t="n">
+      <c r="H24" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="9" t="n">
+      <c r="J24" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="K24" s="9" t="n">
+      <c r="K24" s="8" t="n">
         <v>15</v>
       </c>
       <c r="L24" s="4" t="s">
@@ -3199,10 +3255,10 @@
       <c r="F25" s="6" t="n">
         <v>44997</v>
       </c>
-      <c r="G25" s="8" t="n">
+      <c r="G25" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="H25" s="8" t="n">
+      <c r="H25" s="7" t="n">
         <v>0.729166666666667</v>
       </c>
       <c r="I25" s="4" t="s">
@@ -3242,7 +3298,7 @@
       <c r="I26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="9" t="n">
+      <c r="J26" s="8" t="n">
         <v>10</v>
       </c>
       <c r="K26" s="4" t="s">
@@ -3258,7 +3314,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="103.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>120</v>
       </c>
@@ -3268,15 +3324,19 @@
       <c r="C27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="D27" s="4" t="n">
+        <v>43.110947186732</v>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>-88.5022081314075</v>
+      </c>
       <c r="F27" s="6" t="n">
         <v>44998</v>
       </c>
-      <c r="G27" s="8" t="n">
+      <c r="G27" s="7" t="n">
         <v>0.635416666666667</v>
       </c>
-      <c r="H27" s="8" t="n">
+      <c r="H27" s="7" t="n">
         <v>0.71875</v>
       </c>
       <c r="I27" s="4" t="s">
@@ -3313,10 +3373,10 @@
       <c r="F28" s="6" t="n">
         <v>44999</v>
       </c>
-      <c r="G28" s="8" t="n">
+      <c r="G28" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H28" s="8" t="n">
+      <c r="H28" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I28" s="4" t="s">
@@ -3338,7 +3398,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>130</v>
       </c>
@@ -3348,15 +3408,19 @@
       <c r="C29" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="D29" s="4" t="n">
+        <v>43.0153629744303</v>
+      </c>
+      <c r="E29" s="9" t="n">
+        <v>-88.3110576448882</v>
+      </c>
       <c r="F29" s="6" t="n">
         <v>44999</v>
       </c>
-      <c r="G29" s="8" t="n">
+      <c r="G29" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H29" s="8" t="n">
+      <c r="H29" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I29" s="4" t="s">
@@ -3378,7 +3442,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>136</v>
       </c>
@@ -3388,24 +3452,28 @@
       <c r="C30" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="D30" s="4" t="n">
+        <v>43.1260178587652</v>
+      </c>
+      <c r="E30" s="9" t="n">
+        <v>-88.4628702025553</v>
+      </c>
       <c r="F30" s="6" t="n">
         <v>45000</v>
       </c>
-      <c r="G30" s="8" t="n">
+      <c r="G30" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H30" s="8" t="n">
+      <c r="H30" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="9" t="n">
+      <c r="J30" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K30" s="9" t="n">
+      <c r="K30" s="8" t="n">
         <v>6</v>
       </c>
       <c r="L30" s="4" t="s">
@@ -3418,7 +3486,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>140</v>
       </c>
@@ -3428,15 +3496,19 @@
       <c r="C31" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="D31" s="4" t="n">
+        <v>43.0854162916281</v>
+      </c>
+      <c r="E31" s="9" t="n">
+        <v>-88.0682813160496</v>
+      </c>
       <c r="F31" s="6" t="n">
         <v>45000</v>
       </c>
-      <c r="G31" s="8" t="n">
+      <c r="G31" s="7" t="n">
         <v>0.53125</v>
       </c>
-      <c r="H31" s="8" t="n">
+      <c r="H31" s="7" t="n">
         <v>0.572916666666667</v>
       </c>
       <c r="I31" s="4" t="s">
@@ -3458,7 +3530,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>145</v>
       </c>
@@ -3468,15 +3540,19 @@
       <c r="C32" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="D32" s="4" t="n">
+        <v>43.4228233720421</v>
+      </c>
+      <c r="E32" s="9" t="n">
+        <v>-88.1805872602148</v>
+      </c>
       <c r="F32" s="6" t="n">
         <v>45000</v>
       </c>
-      <c r="G32" s="8" t="n">
+      <c r="G32" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H32" s="8" t="n">
+      <c r="H32" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I32" s="4" t="s">
@@ -3513,10 +3589,10 @@
       <c r="F33" s="6" t="n">
         <v>45001</v>
       </c>
-      <c r="G33" s="8" t="n">
+      <c r="G33" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H33" s="8" t="n">
+      <c r="H33" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
       <c r="I33" s="4" t="s">
@@ -3553,10 +3629,10 @@
       <c r="F34" s="6" t="n">
         <v>45002</v>
       </c>
-      <c r="G34" s="8" t="n">
+      <c r="G34" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H34" s="8" t="n">
+      <c r="H34" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I34" s="4" t="s">
@@ -3565,7 +3641,7 @@
       <c r="J34" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="K34" s="9" t="n">
+      <c r="K34" s="8" t="n">
         <v>20</v>
       </c>
       <c r="L34" s="4" t="s">
@@ -3593,19 +3669,19 @@
       <c r="F35" s="6" t="n">
         <v>45002</v>
       </c>
-      <c r="G35" s="8" t="n">
+      <c r="G35" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="H35" s="8" t="n">
+      <c r="H35" s="7" t="n">
         <v>0.5625</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="9" t="n">
+      <c r="J35" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="K35" s="9" t="n">
+      <c r="K35" s="8" t="n">
         <v>20</v>
       </c>
       <c r="L35" s="4" t="s">
@@ -3633,10 +3709,10 @@
       <c r="F36" s="6" t="n">
         <v>45005</v>
       </c>
-      <c r="G36" s="8" t="n">
+      <c r="G36" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="H36" s="8" t="n">
+      <c r="H36" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="I36" s="4" t="s">
@@ -3669,10 +3745,10 @@
       <c r="F37" s="6" t="n">
         <v>45005</v>
       </c>
-      <c r="G37" s="9" t="n">
+      <c r="G37" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="H37" s="9" t="n">
+      <c r="H37" s="8" t="n">
         <v>12</v>
       </c>
       <c r="I37" s="4" t="s">
@@ -3709,10 +3785,10 @@
       <c r="F38" s="6" t="n">
         <v>45006</v>
       </c>
-      <c r="G38" s="8" t="n">
+      <c r="G38" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H38" s="8" t="n">
+      <c r="H38" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I38" s="4" t="s">
@@ -3749,19 +3825,19 @@
       <c r="F39" s="6" t="n">
         <v>45006</v>
       </c>
-      <c r="G39" s="8" t="n">
+      <c r="G39" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H39" s="8" t="n">
+      <c r="H39" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J39" s="9" t="n">
+      <c r="J39" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="K39" s="9" t="n">
+      <c r="K39" s="8" t="n">
         <v>40</v>
       </c>
       <c r="L39" s="4" t="s">
@@ -3789,19 +3865,19 @@
       <c r="F40" s="6" t="n">
         <v>45007</v>
       </c>
-      <c r="G40" s="8" t="n">
+      <c r="G40" s="7" t="n">
         <v>0.53125</v>
       </c>
-      <c r="H40" s="8" t="n">
+      <c r="H40" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J40" s="9" t="n">
+      <c r="J40" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="K40" s="9" t="n">
+      <c r="K40" s="8" t="n">
         <v>4</v>
       </c>
       <c r="L40" s="4" t="s">
@@ -3829,16 +3905,16 @@
       <c r="F41" s="6" t="n">
         <v>45008</v>
       </c>
-      <c r="G41" s="8" t="n">
+      <c r="G41" s="7" t="n">
         <v>0.833333333333333</v>
       </c>
-      <c r="H41" s="8" t="n">
+      <c r="H41" s="7" t="n">
         <v>0.888888888888889</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J41" s="9" t="n">
+      <c r="J41" s="8" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="4" t="s">
@@ -3864,15 +3940,19 @@
       <c r="C42" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+      <c r="D42" s="4" t="n">
+        <v>43.110947186732</v>
+      </c>
+      <c r="E42" s="4" t="n">
+        <v>-88.5022081314075</v>
+      </c>
       <c r="F42" s="6" t="n">
         <v>45008</v>
       </c>
-      <c r="G42" s="8" t="n">
+      <c r="G42" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H42" s="8" t="n">
+      <c r="H42" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I42" s="4" t="s">
@@ -3909,10 +3989,10 @@
       <c r="F43" s="6" t="n">
         <v>45008</v>
       </c>
-      <c r="G43" s="8" t="n">
+      <c r="G43" s="7" t="n">
         <v>0.6875</v>
       </c>
-      <c r="H43" s="8" t="n">
+      <c r="H43" s="7" t="n">
         <v>0.75</v>
       </c>
       <c r="I43" s="4" t="s">
@@ -3949,10 +4029,10 @@
       <c r="F44" s="6" t="n">
         <v>45009</v>
       </c>
-      <c r="G44" s="8" t="n">
+      <c r="G44" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H44" s="8" t="n">
+      <c r="H44" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
       <c r="I44" s="4" t="s">
@@ -3989,10 +4069,10 @@
       <c r="F45" s="6" t="n">
         <v>45012</v>
       </c>
-      <c r="G45" s="8" t="n">
+      <c r="G45" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H45" s="8" t="n">
+      <c r="H45" s="7" t="n">
         <v>0.604166666666667</v>
       </c>
       <c r="I45" s="4" t="s">
@@ -4029,10 +4109,10 @@
       <c r="F46" s="6" t="n">
         <v>45012</v>
       </c>
-      <c r="G46" s="8" t="n">
+      <c r="G46" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H46" s="8" t="n">
+      <c r="H46" s="7" t="n">
         <v>0.444444444444444</v>
       </c>
       <c r="I46" s="4" t="s">
@@ -4069,10 +4149,10 @@
       <c r="F47" s="6" t="n">
         <v>45012</v>
       </c>
-      <c r="G47" s="8" t="n">
+      <c r="G47" s="7" t="n">
         <v>0.697916666666667</v>
       </c>
-      <c r="H47" s="8" t="n">
+      <c r="H47" s="7" t="n">
         <v>0.739583333333333</v>
       </c>
       <c r="I47" s="4" t="s">
@@ -4109,10 +4189,10 @@
       <c r="F48" s="6" t="n">
         <v>45013</v>
       </c>
-      <c r="G48" s="8" t="n">
+      <c r="G48" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H48" s="8" t="n">
+      <c r="H48" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I48" s="4" t="s">
@@ -4149,10 +4229,10 @@
       <c r="F49" s="6" t="n">
         <v>45014</v>
       </c>
-      <c r="G49" s="8" t="n">
+      <c r="G49" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H49" s="8" t="n">
+      <c r="H49" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I49" s="14" t="n">
@@ -4184,15 +4264,19 @@
       <c r="C50" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
+      <c r="D50" s="4" t="n">
+        <v>42.886038333602</v>
+      </c>
+      <c r="E50" s="9" t="n">
+        <v>-87.9633897374327</v>
+      </c>
       <c r="F50" s="6" t="n">
         <v>45015</v>
       </c>
-      <c r="G50" s="8" t="n">
+      <c r="G50" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="H50" s="8" t="n">
+      <c r="H50" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="I50" s="4" t="s">
@@ -4229,10 +4313,10 @@
       <c r="F51" s="6" t="n">
         <v>45016</v>
       </c>
-      <c r="G51" s="8" t="n">
+      <c r="G51" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H51" s="8" t="n">
+      <c r="H51" s="7" t="n">
         <v>0.444444444444444</v>
       </c>
       <c r="I51" s="4" t="s">
@@ -4269,10 +4353,10 @@
       <c r="F52" s="6" t="n">
         <v>45019</v>
       </c>
-      <c r="G52" s="8" t="n">
+      <c r="G52" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H52" s="8" t="n">
+      <c r="H52" s="7" t="n">
         <v>0.645833333333333</v>
       </c>
       <c r="I52" s="4" t="s">
@@ -4284,7 +4368,7 @@
       <c r="K52" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="L52" s="9" t="n">
+      <c r="L52" s="8" t="n">
         <v>0</v>
       </c>
       <c r="M52" s="4"/>
@@ -4309,10 +4393,10 @@
       <c r="F53" s="6" t="n">
         <v>45021</v>
       </c>
-      <c r="G53" s="8" t="n">
+      <c r="G53" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H53" s="8" t="n">
+      <c r="H53" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
       <c r="I53" s="4" t="s">
@@ -4349,10 +4433,10 @@
       <c r="F54" s="6" t="n">
         <v>45021</v>
       </c>
-      <c r="G54" s="8" t="n">
+      <c r="G54" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H54" s="8" t="n">
+      <c r="H54" s="7" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="I54" s="4" t="s">
@@ -4389,10 +4473,10 @@
       <c r="F55" s="6" t="n">
         <v>45022</v>
       </c>
-      <c r="G55" s="8" t="n">
+      <c r="G55" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H55" s="8" t="n">
+      <c r="H55" s="7" t="n">
         <v>0.96875</v>
       </c>
       <c r="I55" s="4" t="s">
@@ -4429,10 +4513,10 @@
       <c r="F56" s="6" t="n">
         <v>45023</v>
       </c>
-      <c r="G56" s="8" t="n">
+      <c r="G56" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H56" s="8" t="n">
+      <c r="H56" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I56" s="4" t="s">
@@ -4469,19 +4553,19 @@
       <c r="F57" s="6" t="n">
         <v>45026</v>
       </c>
-      <c r="G57" s="8" t="n">
+      <c r="G57" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H57" s="8" t="n">
+      <c r="H57" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="J57" s="9" t="n">
+      <c r="J57" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K57" s="9" t="n">
+      <c r="K57" s="8" t="n">
         <v>40</v>
       </c>
       <c r="L57" s="4" t="s">
@@ -4509,10 +4593,10 @@
       <c r="F58" s="6" t="n">
         <v>45028</v>
       </c>
-      <c r="G58" s="8" t="n">
+      <c r="G58" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H58" s="8" t="n">
+      <c r="H58" s="7" t="n">
         <v>0.46875</v>
       </c>
       <c r="I58" s="4" t="s">
@@ -4549,10 +4633,10 @@
       <c r="F59" s="6" t="n">
         <v>45028</v>
       </c>
-      <c r="G59" s="8" t="n">
+      <c r="G59" s="7" t="n">
         <v>0.53125</v>
       </c>
-      <c r="H59" s="8" t="n">
+      <c r="H59" s="7" t="n">
         <v>0.572916666666667</v>
       </c>
       <c r="I59" s="4" t="s">
@@ -4589,10 +4673,10 @@
       <c r="F60" s="6" t="n">
         <v>45028</v>
       </c>
-      <c r="G60" s="8" t="n">
+      <c r="G60" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H60" s="8" t="n">
+      <c r="H60" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I60" s="4" t="s">
@@ -4629,19 +4713,19 @@
       <c r="F61" s="6" t="n">
         <v>45028</v>
       </c>
-      <c r="G61" s="8" t="n">
+      <c r="G61" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H61" s="8" t="n">
+      <c r="H61" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J61" s="9" t="n">
+      <c r="J61" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K61" s="9" t="n">
+      <c r="K61" s="8" t="n">
         <v>10</v>
       </c>
       <c r="L61" s="4" t="s">
@@ -4669,19 +4753,19 @@
       <c r="F62" s="6" t="n">
         <v>45029</v>
       </c>
-      <c r="G62" s="8" t="n">
+      <c r="G62" s="7" t="n">
         <v>0.375</v>
       </c>
-      <c r="H62" s="8" t="n">
+      <c r="H62" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J62" s="9" t="n">
+      <c r="J62" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="K62" s="9" t="n">
+      <c r="K62" s="8" t="n">
         <v>18</v>
       </c>
       <c r="L62" s="4" t="s">
@@ -4709,10 +4793,10 @@
       <c r="F63" s="6" t="n">
         <v>45030</v>
       </c>
-      <c r="G63" s="8" t="n">
+      <c r="G63" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H63" s="8" t="n">
+      <c r="H63" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I63" s="4"/>
@@ -4722,7 +4806,7 @@
       <c r="K63" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="L63" s="9" t="n">
+      <c r="L63" s="8" t="n">
         <v>0</v>
       </c>
       <c r="M63" s="4"/>
@@ -4747,10 +4831,10 @@
       <c r="F64" s="6" t="n">
         <v>45030</v>
       </c>
-      <c r="G64" s="8" t="n">
+      <c r="G64" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H64" s="8" t="n">
+      <c r="H64" s="7" t="n">
         <v>0.489583333333333</v>
       </c>
       <c r="I64" s="4" t="s">
@@ -4787,16 +4871,16 @@
       <c r="F65" s="6" t="n">
         <v>45030</v>
       </c>
-      <c r="G65" s="8" t="n">
+      <c r="G65" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="H65" s="8" t="n">
+      <c r="H65" s="7" t="n">
         <v>0.5625</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J65" s="9" t="n">
+      <c r="J65" s="8" t="n">
         <v>7</v>
       </c>
       <c r="K65" s="4" t="s">
@@ -4827,10 +4911,10 @@
       <c r="F66" s="6" t="n">
         <v>45031</v>
       </c>
-      <c r="G66" s="8" t="n">
+      <c r="G66" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="H66" s="8" t="n">
+      <c r="H66" s="7" t="n">
         <v>0.729166666666667</v>
       </c>
       <c r="I66" s="4" t="s">
@@ -4901,10 +4985,10 @@
       <c r="F68" s="6" t="n">
         <v>45034</v>
       </c>
-      <c r="G68" s="8" t="n">
+      <c r="G68" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H68" s="8" t="n">
+      <c r="H68" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I68" s="4" t="s">
@@ -4941,19 +5025,19 @@
       <c r="F69" s="6" t="n">
         <v>45035</v>
       </c>
-      <c r="G69" s="8" t="n">
+      <c r="G69" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H69" s="8" t="n">
+      <c r="H69" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J69" s="9" t="n">
+      <c r="J69" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K69" s="9" t="n">
+      <c r="K69" s="8" t="n">
         <v>12</v>
       </c>
       <c r="L69" s="4" t="s">
@@ -4981,10 +5065,10 @@
       <c r="F70" s="6" t="n">
         <v>45035</v>
       </c>
-      <c r="G70" s="8" t="n">
+      <c r="G70" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
-      <c r="H70" s="8" t="n">
+      <c r="H70" s="7" t="n">
         <v>0.5625</v>
       </c>
       <c r="I70" s="4" t="s">
@@ -5021,19 +5105,19 @@
       <c r="F71" s="6" t="n">
         <v>45035</v>
       </c>
-      <c r="G71" s="8" t="n">
+      <c r="G71" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H71" s="8" t="n">
+      <c r="H71" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="J71" s="9" t="n">
+      <c r="J71" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="K71" s="9" t="n">
+      <c r="K71" s="8" t="n">
         <v>40</v>
       </c>
       <c r="L71" s="4" t="s">
@@ -5061,16 +5145,16 @@
       <c r="F72" s="6" t="n">
         <v>45036</v>
       </c>
-      <c r="G72" s="8" t="n">
+      <c r="G72" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="H72" s="8" t="n">
+      <c r="H72" s="7" t="n">
         <v>0.104166666666667</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J72" s="9" t="n">
+      <c r="J72" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K72" s="4" t="s">
@@ -5109,7 +5193,7 @@
       <c r="J73" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K73" s="9" t="n">
+      <c r="K73" s="8" t="n">
         <v>18</v>
       </c>
       <c r="L73" s="4" t="s">
@@ -5137,10 +5221,10 @@
       <c r="F74" s="6" t="n">
         <v>45037</v>
       </c>
-      <c r="G74" s="8" t="n">
+      <c r="G74" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H74" s="8" t="n">
+      <c r="H74" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I74" s="4" t="s">
@@ -5177,16 +5261,16 @@
       <c r="F75" s="6" t="n">
         <v>45038</v>
       </c>
-      <c r="G75" s="8" t="n">
+      <c r="G75" s="7" t="n">
         <v>0.375</v>
       </c>
-      <c r="H75" s="8" t="n">
+      <c r="H75" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J75" s="9" t="n">
+      <c r="J75" s="8" t="n">
         <v>5</v>
       </c>
       <c r="K75" s="4" t="s">
@@ -5217,10 +5301,10 @@
       <c r="F76" s="6" t="n">
         <v>45040</v>
       </c>
-      <c r="G76" s="8" t="n">
+      <c r="G76" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H76" s="8" t="n">
+      <c r="H76" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I76" s="4" t="s">
@@ -5257,10 +5341,10 @@
       <c r="F77" s="6" t="n">
         <v>45040</v>
       </c>
-      <c r="G77" s="8" t="n">
+      <c r="G77" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H77" s="8" t="n">
+      <c r="H77" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I77" s="4" t="s">
@@ -5297,10 +5381,10 @@
       <c r="F78" s="6" t="n">
         <v>45042</v>
       </c>
-      <c r="G78" s="8" t="n">
+      <c r="G78" s="7" t="n">
         <v>0.364583333333333</v>
       </c>
-      <c r="H78" s="8" t="n">
+      <c r="H78" s="7" t="n">
         <v>0.652777777777778</v>
       </c>
       <c r="I78" s="4" t="s">
@@ -5337,16 +5421,16 @@
       <c r="F79" s="6" t="n">
         <v>45042</v>
       </c>
-      <c r="G79" s="8" t="n">
+      <c r="G79" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H79" s="8" t="n">
+      <c r="H79" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J79" s="9" t="n">
+      <c r="J79" s="8" t="n">
         <v>5</v>
       </c>
       <c r="K79" s="4" t="s">
@@ -5377,16 +5461,16 @@
       <c r="F80" s="6" t="n">
         <v>45044</v>
       </c>
-      <c r="G80" s="8" t="n">
+      <c r="G80" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H80" s="8" t="n">
+      <c r="H80" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J80" s="9" t="n">
+      <c r="J80" s="8" t="n">
         <v>3</v>
       </c>
       <c r="K80" s="4" t="s">
@@ -5417,10 +5501,10 @@
       <c r="F81" s="6" t="n">
         <v>45044</v>
       </c>
-      <c r="G81" s="8" t="n">
+      <c r="G81" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H81" s="8" t="n">
+      <c r="H81" s="7" t="n">
         <v>0.489583333333333</v>
       </c>
       <c r="I81" s="4" t="s">
@@ -5457,10 +5541,10 @@
       <c r="F82" s="6" t="n">
         <v>45044</v>
       </c>
-      <c r="G82" s="8" t="n">
+      <c r="G82" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="H82" s="8" t="n">
+      <c r="H82" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="I82" s="4" t="s">
@@ -5497,10 +5581,10 @@
       <c r="F83" s="6" t="n">
         <v>45047</v>
       </c>
-      <c r="G83" s="8" t="n">
+      <c r="G83" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H83" s="8" t="n">
+      <c r="H83" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I83" s="4" t="s">
@@ -5509,7 +5593,7 @@
       <c r="J83" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="K83" s="9" t="n">
+      <c r="K83" s="8" t="n">
         <v>50</v>
       </c>
       <c r="L83" s="4" t="s">
@@ -5537,22 +5621,22 @@
       <c r="F84" s="6" t="n">
         <v>45047</v>
       </c>
-      <c r="G84" s="8" t="n">
+      <c r="G84" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H84" s="8" t="n">
+      <c r="H84" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I84" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J84" s="9" t="n">
+      <c r="J84" s="8" t="n">
         <v>3</v>
       </c>
       <c r="K84" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L84" s="9" t="n">
+      <c r="L84" s="8" t="n">
         <v>0</v>
       </c>
       <c r="M84" s="4"/>
@@ -5577,16 +5661,16 @@
       <c r="F85" s="6" t="n">
         <v>45048</v>
       </c>
-      <c r="G85" s="8" t="n">
+      <c r="G85" s="7" t="n">
         <v>0.409722222222222</v>
       </c>
-      <c r="H85" s="8" t="n">
+      <c r="H85" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J85" s="9" t="n">
+      <c r="J85" s="8" t="n">
         <v>6</v>
       </c>
       <c r="K85" s="4" t="s">
@@ -5617,10 +5701,10 @@
       <c r="F86" s="6" t="n">
         <v>45048</v>
       </c>
-      <c r="G86" s="8" t="n">
+      <c r="G86" s="7" t="n">
         <v>0.583333333333333</v>
       </c>
-      <c r="H86" s="8" t="n">
+      <c r="H86" s="7" t="n">
         <v>0.645833333333333</v>
       </c>
       <c r="I86" s="4" t="s">
@@ -5657,16 +5741,16 @@
       <c r="F87" s="6" t="n">
         <v>45048</v>
       </c>
-      <c r="G87" s="8" t="n">
+      <c r="G87" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="H87" s="8" t="n">
+      <c r="H87" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="J87" s="9" t="n">
+      <c r="J87" s="8" t="n">
         <v>2</v>
       </c>
       <c r="K87" s="4" t="s">
@@ -5697,10 +5781,10 @@
       <c r="F88" s="6" t="n">
         <v>45049</v>
       </c>
-      <c r="G88" s="8" t="n">
+      <c r="G88" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H88" s="8" t="n">
+      <c r="H88" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
       <c r="I88" s="4" t="s">
@@ -5722,7 +5806,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="307.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
         <v>366</v>
       </c>
@@ -5732,15 +5816,19 @@
       <c r="C89" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
+      <c r="D89" s="4" t="n">
+        <v>42.9588185809146</v>
+      </c>
+      <c r="E89" s="9" t="n">
+        <v>-87.9783010214933</v>
+      </c>
       <c r="F89" s="6" t="n">
         <v>45049</v>
       </c>
-      <c r="G89" s="8" t="n">
+      <c r="G89" s="7" t="n">
         <v>0.53125</v>
       </c>
-      <c r="H89" s="8" t="n">
+      <c r="H89" s="7" t="n">
         <v>0.604166666666667</v>
       </c>
       <c r="I89" s="4" t="s">
@@ -5777,10 +5865,10 @@
       <c r="F90" s="6" t="n">
         <v>45049</v>
       </c>
-      <c r="G90" s="8" t="n">
+      <c r="G90" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H90" s="8" t="n">
+      <c r="H90" s="7" t="n">
         <v>0.427083333333333</v>
       </c>
       <c r="I90" s="4" t="s">
@@ -5802,7 +5890,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
         <v>355</v>
       </c>
@@ -5812,21 +5900,25 @@
       <c r="C91" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
+      <c r="D91" s="4" t="n">
+        <v>42.9588185809146</v>
+      </c>
+      <c r="E91" s="9" t="n">
+        <v>-87.9783010214933</v>
+      </c>
       <c r="F91" s="6" t="n">
         <v>45049</v>
       </c>
-      <c r="G91" s="8" t="n">
+      <c r="G91" s="7" t="n">
         <v>0.489583333333333</v>
       </c>
-      <c r="H91" s="8" t="n">
+      <c r="H91" s="7" t="n">
         <v>0.53125</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="J91" s="9" t="n">
+      <c r="J91" s="8" t="n">
         <v>2</v>
       </c>
       <c r="K91" s="4" t="s">
@@ -5842,7 +5934,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
         <v>376</v>
       </c>
@@ -5852,15 +5944,19 @@
       <c r="C92" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
+      <c r="D92" s="4" t="n">
+        <v>42.9588185809146</v>
+      </c>
+      <c r="E92" s="9" t="n">
+        <v>-87.9783010214933</v>
+      </c>
       <c r="F92" s="6" t="n">
         <v>45049</v>
       </c>
-      <c r="G92" s="8" t="n">
+      <c r="G92" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="H92" s="8" t="n">
+      <c r="H92" s="7" t="n">
         <v>0.53125</v>
       </c>
       <c r="I92" s="4" t="s">
@@ -5897,10 +5993,10 @@
       <c r="F93" s="6" t="n">
         <v>45050</v>
       </c>
-      <c r="G93" s="8" t="n">
+      <c r="G93" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H93" s="8" t="n">
+      <c r="H93" s="7" t="n">
         <v>0.46875</v>
       </c>
       <c r="I93" s="4" t="s">
@@ -5937,10 +6033,10 @@
       <c r="F94" s="6" t="n">
         <v>45051</v>
       </c>
-      <c r="G94" s="8" t="n">
+      <c r="G94" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H94" s="8" t="n">
+      <c r="H94" s="7" t="n">
         <v>0.604166666666667</v>
       </c>
       <c r="I94" s="4" t="s">
@@ -5977,19 +6073,19 @@
       <c r="F95" s="6" t="n">
         <v>45051</v>
       </c>
-      <c r="G95" s="8" t="n">
+      <c r="G95" s="7" t="n">
         <v>0.375</v>
       </c>
-      <c r="H95" s="8" t="n">
+      <c r="H95" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I95" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="J95" s="9" t="n">
+      <c r="J95" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K95" s="9" t="n">
+      <c r="K95" s="8" t="n">
         <v>60</v>
       </c>
       <c r="L95" s="4" t="s">
@@ -6017,10 +6113,10 @@
       <c r="F96" s="6" t="n">
         <v>45052</v>
       </c>
-      <c r="G96" s="8" t="n">
+      <c r="G96" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H96" s="8" t="n">
+      <c r="H96" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="I96" s="4" t="s">
@@ -6057,22 +6153,22 @@
       <c r="F97" s="6" t="n">
         <v>45054</v>
       </c>
-      <c r="G97" s="8" t="n">
+      <c r="G97" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H97" s="8" t="n">
+      <c r="H97" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J97" s="9" t="n">
+      <c r="J97" s="8" t="n">
         <v>3</v>
       </c>
       <c r="K97" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="L97" s="9" t="n">
+      <c r="L97" s="8" t="n">
         <v>0</v>
       </c>
       <c r="M97" s="4"/>
@@ -6097,16 +6193,16 @@
       <c r="F98" s="6" t="n">
         <v>45054</v>
       </c>
-      <c r="G98" s="8" t="n">
+      <c r="G98" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H98" s="8" t="n">
+      <c r="H98" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I98" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J98" s="9" t="n">
+      <c r="J98" s="8" t="n">
         <v>8</v>
       </c>
       <c r="K98" s="4" t="s">
@@ -6137,19 +6233,19 @@
       <c r="F99" s="6" t="n">
         <v>45055</v>
       </c>
-      <c r="G99" s="8" t="n">
+      <c r="G99" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H99" s="8" t="n">
+      <c r="H99" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J99" s="9" t="n">
+      <c r="J99" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="K99" s="9" t="n">
+      <c r="K99" s="8" t="n">
         <v>20</v>
       </c>
       <c r="L99" s="4" t="s">
@@ -6177,10 +6273,10 @@
       <c r="F100" s="6" t="n">
         <v>45056</v>
       </c>
-      <c r="G100" s="8" t="n">
+      <c r="G100" s="7" t="n">
         <v>0.53125</v>
       </c>
-      <c r="H100" s="8" t="n">
+      <c r="H100" s="7" t="n">
         <v>0.572916666666667</v>
       </c>
       <c r="I100" s="4" t="s">
@@ -6217,10 +6313,10 @@
       <c r="F101" s="6" t="n">
         <v>45056</v>
       </c>
-      <c r="G101" s="8" t="n">
+      <c r="G101" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H101" s="8" t="n">
+      <c r="H101" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I101" s="4" t="s">
@@ -6252,15 +6348,19 @@
       <c r="C102" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="D102" s="4"/>
-      <c r="E102" s="4"/>
+      <c r="D102" s="4" t="n">
+        <v>42.886038333602</v>
+      </c>
+      <c r="E102" s="9" t="n">
+        <v>-87.9633897374327</v>
+      </c>
       <c r="F102" s="6" t="n">
         <v>45057</v>
       </c>
-      <c r="G102" s="8" t="n">
+      <c r="G102" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H102" s="8" t="n">
+      <c r="H102" s="7" t="n">
         <v>0.625</v>
       </c>
       <c r="I102" s="4" t="s">
@@ -6297,14 +6397,14 @@
       <c r="F103" s="6" t="n">
         <v>45058</v>
       </c>
-      <c r="G103" s="8" t="n">
+      <c r="G103" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H103" s="8" t="n">
+      <c r="H103" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I103" s="4"/>
-      <c r="J103" s="9" t="n">
+      <c r="J103" s="8" t="n">
         <v>2</v>
       </c>
       <c r="K103" s="4" t="s">
@@ -6335,10 +6435,10 @@
       <c r="F104" s="6" t="n">
         <v>45059</v>
       </c>
-      <c r="G104" s="8" t="n">
+      <c r="G104" s="7" t="n">
         <v>0.5625</v>
       </c>
-      <c r="H104" s="8" t="n">
+      <c r="H104" s="7" t="n">
         <v>0.645833333333333</v>
       </c>
       <c r="I104" s="4" t="s">
@@ -6375,19 +6475,19 @@
       <c r="F105" s="6" t="n">
         <v>45061</v>
       </c>
-      <c r="G105" s="8" t="n">
+      <c r="G105" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H105" s="8" t="n">
+      <c r="H105" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I105" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J105" s="9" t="n">
+      <c r="J105" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K105" s="9" t="n">
+      <c r="K105" s="8" t="n">
         <v>7</v>
       </c>
       <c r="L105" s="4" t="s">
@@ -6415,10 +6515,10 @@
       <c r="F106" s="6" t="n">
         <v>45062</v>
       </c>
-      <c r="G106" s="8" t="n">
+      <c r="G106" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H106" s="8" t="n">
+      <c r="H106" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I106" s="4" t="s">
@@ -6455,19 +6555,19 @@
       <c r="F107" s="6" t="n">
         <v>45063</v>
       </c>
-      <c r="G107" s="8" t="n">
+      <c r="G107" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H107" s="8" t="n">
+      <c r="H107" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
       <c r="I107" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J107" s="9" t="n">
+      <c r="J107" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K107" s="9" t="n">
+      <c r="K107" s="8" t="n">
         <v>10</v>
       </c>
       <c r="L107" s="4" t="s">
@@ -6495,10 +6595,10 @@
       <c r="F108" s="6" t="n">
         <v>45063</v>
       </c>
-      <c r="G108" s="8" t="n">
+      <c r="G108" s="7" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="H108" s="8" t="n">
+      <c r="H108" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="I108" s="4" t="s">
@@ -6520,7 +6620,7 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
         <v>442</v>
       </c>
@@ -6530,15 +6630,19 @@
       <c r="C109" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
+      <c r="D109" s="4" t="n">
+        <v>42.886038333602</v>
+      </c>
+      <c r="E109" s="9" t="n">
+        <v>-87.9633897374327</v>
+      </c>
       <c r="F109" s="6" t="n">
         <v>45064</v>
       </c>
-      <c r="G109" s="8" t="n">
+      <c r="G109" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H109" s="8" t="n">
+      <c r="H109" s="7" t="n">
         <v>0.604166666666667</v>
       </c>
       <c r="I109" s="4" t="s">
@@ -6575,22 +6679,22 @@
       <c r="F110" s="6" t="n">
         <v>45064</v>
       </c>
-      <c r="G110" s="8" t="n">
+      <c r="G110" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="H110" s="8" t="n">
+      <c r="H110" s="7" t="n">
         <v>0.75</v>
       </c>
       <c r="I110" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J110" s="9" t="n">
+      <c r="J110" s="8" t="n">
         <v>1</v>
       </c>
       <c r="K110" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L110" s="9" t="n">
+      <c r="L110" s="8" t="n">
         <v>0</v>
       </c>
       <c r="M110" s="4"/>
@@ -6615,10 +6719,10 @@
       <c r="F111" s="6" t="n">
         <v>45065</v>
       </c>
-      <c r="G111" s="8" t="n">
+      <c r="G111" s="7" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="H111" s="8" t="n">
+      <c r="H111" s="7" t="n">
         <v>0.833333333333333</v>
       </c>
       <c r="I111" s="4" t="s">
@@ -6655,19 +6759,19 @@
       <c r="F112" s="6" t="n">
         <v>45065</v>
       </c>
-      <c r="G112" s="8" t="n">
+      <c r="G112" s="7" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="H112" s="8" t="n">
+      <c r="H112" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I112" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="J112" s="9" t="n">
+      <c r="J112" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="K112" s="9" t="n">
+      <c r="K112" s="8" t="n">
         <v>25</v>
       </c>
       <c r="L112" s="4" t="s">
@@ -6695,10 +6799,10 @@
       <c r="F113" s="6" t="n">
         <v>45066</v>
       </c>
-      <c r="G113" s="8" t="n">
+      <c r="G113" s="7" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="H113" s="8" t="n">
+      <c r="H113" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
       <c r="I113" s="4" t="s">
@@ -6733,10 +6837,10 @@
       <c r="F114" s="6" t="n">
         <v>45068</v>
       </c>
-      <c r="G114" s="8" t="n">
+      <c r="G114" s="7" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="H114" s="8" t="n">
+      <c r="H114" s="7" t="n">
         <v>0.572916666666667</v>
       </c>
       <c r="I114" s="4" t="s">
@@ -6773,10 +6877,10 @@
       <c r="F115" s="6" t="n">
         <v>45068</v>
       </c>
-      <c r="G115" s="8" t="n">
+      <c r="G115" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="H115" s="8" t="n">
+      <c r="H115" s="7" t="n">
         <v>0.729166666666667</v>
       </c>
       <c r="I115" s="4" t="s">
@@ -6813,10 +6917,10 @@
       <c r="F116" s="6" t="n">
         <v>45068</v>
       </c>
-      <c r="G116" s="8" t="n">
+      <c r="G116" s="7" t="n">
         <v>0.625</v>
       </c>
-      <c r="H116" s="8" t="n">
+      <c r="H116" s="7" t="n">
         <v>0.999305555555556</v>
       </c>
       <c r="I116" s="4" t="s">
@@ -6853,10 +6957,10 @@
       <c r="F117" s="6" t="n">
         <v>45069</v>
       </c>
-      <c r="G117" s="8" t="n">
+      <c r="G117" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H117" s="8" t="n">
+      <c r="H117" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I117" s="4" t="s">
@@ -6893,10 +6997,10 @@
       <c r="F118" s="6" t="n">
         <v>45069</v>
       </c>
-      <c r="G118" s="8" t="n">
+      <c r="G118" s="7" t="n">
         <v>0.520833333333333</v>
       </c>
-      <c r="H118" s="8" t="n">
+      <c r="H118" s="7" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="I118" s="4" t="s">
@@ -6933,10 +7037,10 @@
       <c r="F119" s="6" t="n">
         <v>45069</v>
       </c>
-      <c r="G119" s="8" t="n">
+      <c r="G119" s="7" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="H119" s="8" t="n">
+      <c r="H119" s="7" t="n">
         <v>0.833333333333333</v>
       </c>
       <c r="I119" s="4" t="s">
@@ -6973,16 +7077,16 @@
       <c r="F120" s="6" t="n">
         <v>45070</v>
       </c>
-      <c r="G120" s="8" t="n">
+      <c r="G120" s="7" t="n">
         <v>0.416666666666667</v>
       </c>
-      <c r="H120" s="8" t="n">
+      <c r="H120" s="7" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="I120" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J120" s="9" t="n">
+      <c r="J120" s="8" t="n">
         <v>1</v>
       </c>
       <c r="K120" s="4" t="s">
@@ -7013,10 +7117,10 @@
       <c r="F121" s="6" t="n">
         <v>45070</v>
       </c>
-      <c r="G121" s="8" t="n">
+      <c r="G121" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H121" s="8" t="n">
+      <c r="H121" s="7" t="n">
         <v>0.46875</v>
       </c>
       <c r="I121" s="4" t="s">
@@ -7053,10 +7157,10 @@
       <c r="F122" s="6" t="n">
         <v>45072</v>
       </c>
-      <c r="G122" s="8" t="n">
+      <c r="G122" s="7" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="H122" s="8" t="n">
+      <c r="H122" s="7" t="n">
         <v>0.833333333333333</v>
       </c>
       <c r="I122" s="4" t="s">
@@ -7093,16 +7197,16 @@
       <c r="F123" s="6" t="n">
         <v>45075</v>
       </c>
-      <c r="G123" s="8" t="n">
+      <c r="G123" s="7" t="n">
         <v>0.604166666666667</v>
       </c>
-      <c r="H123" s="8" t="n">
+      <c r="H123" s="7" t="n">
         <v>0.65625</v>
       </c>
       <c r="I123" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J123" s="9" t="n">
+      <c r="J123" s="8" t="n">
         <v>20</v>
       </c>
       <c r="K123" s="4" t="s">
@@ -7133,10 +7237,10 @@
       <c r="F124" s="6" t="n">
         <v>45076</v>
       </c>
-      <c r="G124" s="8" t="n">
+      <c r="G124" s="7" t="n">
         <v>0.4375</v>
       </c>
-      <c r="H124" s="8" t="n">
+      <c r="H124" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="I124" s="4" t="s">

</xml_diff>